<commit_message>
Hybrid Driven Framework - Complete
</commit_message>
<xml_diff>
--- a/HybridFramework/src/testData/TestData.xlsx
+++ b/HybridFramework/src/testData/TestData.xlsx
@@ -3,21 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://boozallen-my.sharepoint.com/personal/625337_bah_com/Documents/Documents/Personal/Trainings/Selenium/Workspaces/Feb2023/HybridFramework/src/testData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\625337\OneDrive - BOOZ ALLEN HAMILTON\Documents\Personal\Trainings\Selenium\Workspaces\Feb2023\HybridFramework\src\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{BDDAA33E-A653-4026-845F-61CDA895F768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1C9450D-59D3-47E2-B97A-43430EDD28D6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F953A65A-FB30-4299-B5BF-C773B0ED1E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{40914548-F9A3-4D3F-B989-9A3EE95A24BE}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{40914548-F9A3-4D3F-B989-9A3EE95A24BE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Test-Data" sheetId="2" r:id="rId1"/>
+    <sheet name="Test Cases" sheetId="3" r:id="rId1"/>
+    <sheet name="Test-Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -58,13 +59,77 @@
   </si>
   <si>
     <t>Chrome</t>
+  </si>
+  <si>
+    <t>Product Type</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Framework_001</t>
+  </si>
+  <si>
+    <t>Framework_002</t>
+  </si>
+  <si>
+    <t>chuy2@bah.com</t>
+  </si>
+  <si>
+    <t>fashion</t>
+  </si>
+  <si>
+    <t>Edge</t>
+  </si>
+  <si>
+    <t>Framework_003</t>
+  </si>
+  <si>
+    <t>anshika@gmail.com</t>
+  </si>
+  <si>
+    <t>Iamking@000</t>
+  </si>
+  <si>
+    <t>Mozilla</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>ADIDAS ORIGINAL</t>
+  </si>
+  <si>
+    <t>ZARA COAT 3</t>
+  </si>
+  <si>
+    <t>electronics</t>
+  </si>
+  <si>
+    <t>IPHONE 13 PRO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,6 +141,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -119,15 +192,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -439,19 +515,154 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8BEA1D9-5F7D-4D77-9A38-69F706871355}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="21.7109375"/>
+    <col min="2" max="2" customWidth="true" width="20.0"/>
+    <col min="3" max="3" customWidth="true" width="16.0"/>
+    <col min="4" max="4" customWidth="true" width="13.140625"/>
+    <col min="5" max="5" customWidth="true" width="20.0"/>
+    <col min="6" max="6" customWidth="true" width="22.0"/>
+    <col min="7" max="7" customWidth="true" width="16.7109375"/>
+    <col min="8" max="8" customWidth="true" width="17.28515625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{73F59A9E-FCE8-4F0F-96B5-99D13F4C27DF}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{8EAD6AE2-87A6-4602-91B3-64FB6FE1E0BD}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{464468F7-96D6-473B-94DE-D961C7733BF6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4F97B8-C1E6-4777-A6D6-7948174E4994}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="21.7109375"/>
+    <col min="2" max="2" customWidth="true" width="20.0"/>
+    <col min="3" max="3" customWidth="true" width="16.0"/>
+    <col min="4" max="4" customWidth="true" width="13.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>